<commit_message>
fix: Improve comments for clarity and consistency across multiple files
fix: Improve comments for clarity and consistency across multiple files
</commit_message>
<xml_diff>
--- a/docs/Plan de pruebas.xlsx
+++ b/docs/Plan de pruebas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://udcgal-my.sharepoint.com/personal/sebastian_exposito_udc_es/Documents/Documentos/Universidad (materias)/2do curso/1er cuatri/IS/p/p-is-repo/Proyecto_IS/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alvar\OneDrive\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A24F9C1-2382-0945-B977-65EAD374CCF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EB4070A-7684-4A1C-BBB9-7A6F163DF874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="940" windowWidth="29080" windowHeight="18040" xr2:uid="{34238E7A-1763-481E-87A2-76BE29C62A4F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{34238E7A-1763-481E-87A2-76BE29C62A4F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="150">
   <si>
     <t>ID</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>Resultado Esperado (DoD)</t>
+  </si>
+  <si>
+    <t>Tipo</t>
   </si>
   <si>
     <t>Estado</t>
@@ -133,6 +136,9 @@
     <t>2. Verificar el filtro de extensiones.</t>
   </si>
   <si>
+    <t>El explorador solo permite seleccionar archivos compatibles (CSV, Excel, SQLite).</t>
+  </si>
+  <si>
     <t>TC-03</t>
   </si>
   <si>
@@ -642,6 +648,24 @@
     <t>Mensaje de error: "Missing value" o "Invalid numeric value".</t>
   </si>
   <si>
+    <t>Positivo</t>
+  </si>
+  <si>
+    <t>Negativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Visual</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Negativo</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Positivo</t>
+  </si>
+  <si>
+    <t>tick</t>
+  </si>
+  <si>
     <t>El sistema muestra un mensaje de error claro y no se cierra (No crash).</t>
   </si>
   <si>
@@ -692,33 +716,28 @@
     </r>
   </si>
   <si>
-    <t>El explorador permite seleccionar archivos compatibles (CSV, Excel, SQLite).</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Intentar cargar un </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF444746"/>
-        <rFont val="Google Sans Text"/>
-        <family val="2"/>
-      </rPr>
-      <t>.joblib</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF1F1F1F"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> roto/vacio.</t>
-    </r>
-  </si>
-  <si>
-    <t>TC -&gt; Test Case</t>
+    <t>1. Intentar cargar un .joblib roto</t>
+  </si>
+  <si>
+    <t>SECCIÓN PREPROCESADO</t>
+  </si>
+  <si>
+    <t>SELECCIÓN DE COLUMNAS</t>
+  </si>
+  <si>
+    <t>DIVISIÓN DE DATOS</t>
+  </si>
+  <si>
+    <t>CREACIÓN Y VISUALIZACIÓN MODELO</t>
+  </si>
+  <si>
+    <t>DESCRIPCIÓN Y GUARDADO</t>
+  </si>
+  <si>
+    <t>CARGAR MODELO</t>
+  </si>
+  <si>
+    <t>PREDICCIONES</t>
   </si>
 </sst>
 </file>
@@ -818,7 +837,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
@@ -844,38 +863,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-      <extLst>
-        <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
-          <xfpb:xfComplement i="0"/>
-        </ext>
-      </extLst>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -893,25 +880,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/featurePropertyBag/featurePropertyBag.xml><?xml version="1.0" encoding="utf-8"?>
-<FeaturePropertyBags xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag">
-  <bag type="Checkbox"/>
-  <bag type="XFControls">
-    <bagId k="CellControl">0</bagId>
-  </bag>
-  <bag type="XFComplement">
-    <bagId k="XFControls">1</bagId>
-  </bag>
-  <bag type="XFComplements" extRef="XFComplementsMapperExtRef">
-    <a k="MappedFeaturePropertyBags">
-      <bagId>2</bagId>
-    </a>
-  </bag>
-</FeaturePropertyBags>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1227,22 +1197,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E40F15B-D907-4584-927D-29DD0F472893}">
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="163" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="29.5" customWidth="1"/>
-    <col min="3" max="3" width="23.83203125" customWidth="1"/>
-    <col min="4" max="4" width="25.83203125" customWidth="1"/>
-    <col min="5" max="5" width="13.5" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.44140625" customWidth="1"/>
+    <col min="3" max="3" width="23.88671875" customWidth="1"/>
+    <col min="4" max="4" width="25.77734375" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="16" thickBot="1">
+    <row r="1" spans="1:6" ht="15" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1258,140 +1227,163 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1">
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="9" t="b">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>10</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="7"/>
       <c r="B3" s="7"/>
       <c r="C3" s="4"/>
       <c r="D3" s="7"/>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:7" ht="31" thickBot="1">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" ht="28.2" thickBot="1">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:6" ht="54" customHeight="1">
+      <c r="A5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="11"/>
-    </row>
-    <row r="5" spans="1:7" ht="54" customHeight="1">
-      <c r="A5" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D5" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="E5" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="7"/>
-      <c r="E6" s="10"/>
-    </row>
-    <row r="7" spans="1:7" ht="31" thickBot="1">
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" ht="28.2" thickBot="1">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="11"/>
-    </row>
-    <row r="8" spans="1:7" ht="30" customHeight="1">
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+    </row>
+    <row r="8" spans="1:6" ht="27.6">
       <c r="A8" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>132</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="4"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="10"/>
-    </row>
-    <row r="10" spans="1:7" ht="31" thickBot="1">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" ht="28.2" thickBot="1">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D10" s="8"/>
-      <c r="E10" s="11"/>
-    </row>
-    <row r="11" spans="1:7" ht="46" thickBot="1">
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:6" ht="42" thickBot="1">
       <c r="A11" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="E11" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>133</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12" s="5"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" ht="16" thickBot="1">
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" ht="15" thickBot="1">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="C13" s="5" t="s">
+        <v>144</v>
+      </c>
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" ht="16" thickBot="1">
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:6" ht="15" thickBot="1">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
@@ -1407,154 +1399,181 @@
       <c r="E14" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" ht="40.25" customHeight="1">
+      <c r="F14" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="40.200000000000003" customHeight="1">
       <c r="A15" s="6" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>26</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="4"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="10"/>
-    </row>
-    <row r="17" spans="1:5" ht="31" thickBot="1">
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" ht="28.2" thickBot="1">
       <c r="A17" s="8"/>
       <c r="B17" s="8"/>
       <c r="C17" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="11"/>
-    </row>
-    <row r="18" spans="1:5" ht="30">
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" ht="27.6">
       <c r="A18" s="6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="D18" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E18" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+      <c r="F18" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="4"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="10"/>
-    </row>
-    <row r="20" spans="1:5" ht="31" thickBot="1">
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+    </row>
+    <row r="20" spans="1:6" ht="28.2" thickBot="1">
       <c r="A20" s="8"/>
       <c r="B20" s="8"/>
       <c r="C20" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D20" s="8"/>
-      <c r="E20" s="11"/>
-    </row>
-    <row r="21" spans="1:5" ht="30">
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" ht="27.6">
       <c r="A21" s="6" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B21" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E21" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
+      <c r="E21" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="4"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="10"/>
-    </row>
-    <row r="23" spans="1:5" ht="31" thickBot="1">
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
+    </row>
+    <row r="23" spans="1:6" ht="28.2" thickBot="1">
       <c r="A23" s="8"/>
       <c r="B23" s="8"/>
       <c r="C23" s="2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D23" s="8"/>
-      <c r="E23" s="11"/>
-    </row>
-    <row r="24" spans="1:5" ht="30">
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" ht="27.6">
       <c r="A24" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E24" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
+        <v>37</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="4"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="10"/>
-    </row>
-    <row r="26" spans="1:5" ht="16" thickBot="1">
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" ht="28.2" thickBot="1">
       <c r="A26" s="8"/>
       <c r="B26" s="8"/>
       <c r="C26" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D26" s="8"/>
-      <c r="E26" s="11"/>
-    </row>
-    <row r="27" spans="1:5">
+      <c r="E26" s="8"/>
+      <c r="F26" s="8"/>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" s="5"/>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
-    </row>
-    <row r="28" spans="1:5" ht="16" thickBot="1">
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="1:6" ht="15" thickBot="1">
       <c r="A28" s="5"/>
       <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>143</v>
+      </c>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
-    </row>
-    <row r="29" spans="1:5" ht="16" thickBot="1">
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="1:6" ht="15" thickBot="1">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
@@ -1570,154 +1589,181 @@
       <c r="E29" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="30">
+      <c r="F29" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="27.6">
       <c r="A30" s="6" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
+        <v>42</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31" s="7"/>
       <c r="B31" s="7"/>
       <c r="C31" s="4"/>
       <c r="D31" s="7"/>
-      <c r="E31" s="10"/>
-    </row>
-    <row r="32" spans="1:5" ht="16" thickBot="1">
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" ht="15" thickBot="1">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D32" s="8"/>
-      <c r="E32" s="11"/>
-    </row>
-    <row r="33" spans="1:5" ht="30">
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+    </row>
+    <row r="33" spans="1:6" ht="27.6">
       <c r="A33" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E33" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5">
+        <v>46</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34" s="7"/>
       <c r="B34" s="7"/>
       <c r="C34" s="4"/>
       <c r="D34" s="7"/>
-      <c r="E34" s="10"/>
-    </row>
-    <row r="35" spans="1:5" ht="16" thickBot="1">
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" ht="15" thickBot="1">
       <c r="A35" s="8"/>
       <c r="B35" s="8"/>
       <c r="C35" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="D35" s="8"/>
-      <c r="E35" s="11"/>
-    </row>
-    <row r="36" spans="1:5" ht="30">
+      <c r="E35" s="8"/>
+      <c r="F35" s="8"/>
+    </row>
+    <row r="36" spans="1:6" ht="27.6">
       <c r="A36" s="6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5">
+        <v>51</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37" s="7"/>
       <c r="B37" s="7"/>
       <c r="C37" s="4"/>
       <c r="D37" s="7"/>
-      <c r="E37" s="10"/>
-    </row>
-    <row r="38" spans="1:5" ht="31" thickBot="1">
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+    </row>
+    <row r="38" spans="1:6" ht="28.2" thickBot="1">
       <c r="A38" s="8"/>
       <c r="B38" s="8"/>
       <c r="C38" s="2" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D38" s="8"/>
-      <c r="E38" s="11"/>
-    </row>
-    <row r="39" spans="1:5" ht="67.75" customHeight="1">
+      <c r="E38" s="8"/>
+      <c r="F38" s="8"/>
+    </row>
+    <row r="39" spans="1:6" ht="67.8" customHeight="1">
       <c r="A39" s="6" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="E39" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5">
+        <v>141</v>
+      </c>
+      <c r="E39" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40" s="7"/>
       <c r="B40" s="7"/>
       <c r="C40" s="4"/>
       <c r="D40" s="7"/>
-      <c r="E40" s="10"/>
-    </row>
-    <row r="41" spans="1:5" ht="16" thickBot="1">
+      <c r="E40" s="7"/>
+      <c r="F40" s="7"/>
+    </row>
+    <row r="41" spans="1:6" ht="15" thickBot="1">
       <c r="A41" s="8"/>
       <c r="B41" s="8"/>
       <c r="C41" s="2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="D41" s="8"/>
-      <c r="E41" s="11"/>
-    </row>
-    <row r="42" spans="1:5">
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42" s="5"/>
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
-    </row>
-    <row r="43" spans="1:5" ht="16" thickBot="1">
+      <c r="F42" s="5"/>
+    </row>
+    <row r="43" spans="1:6" ht="15" thickBot="1">
       <c r="A43" s="5"/>
       <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>145</v>
+      </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
-    </row>
-    <row r="44" spans="1:5" ht="16" thickBot="1">
+      <c r="F43" s="5"/>
+    </row>
+    <row r="44" spans="1:6" ht="15" thickBot="1">
       <c r="A44" s="3" t="s">
         <v>0</v>
       </c>
@@ -1733,122 +1779,145 @@
       <c r="E44" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="30">
+      <c r="F44" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="27.6">
       <c r="A45" s="6" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="E45" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5">
+        <v>136</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46" s="7"/>
       <c r="B46" s="7"/>
       <c r="C46" s="4"/>
       <c r="D46" s="7"/>
-      <c r="E46" s="10"/>
-    </row>
-    <row r="47" spans="1:5" ht="31" thickBot="1">
+      <c r="E46" s="7"/>
+      <c r="F46" s="7"/>
+    </row>
+    <row r="47" spans="1:6" ht="28.2" thickBot="1">
       <c r="A47" s="8"/>
       <c r="B47" s="8"/>
       <c r="C47" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D47" s="8"/>
-      <c r="E47" s="11"/>
-    </row>
-    <row r="48" spans="1:5" ht="46" thickBot="1">
+      <c r="E47" s="8"/>
+      <c r="F47" s="8"/>
+    </row>
+    <row r="48" spans="1:6" ht="42" thickBot="1">
       <c r="A48" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E48" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" ht="30">
+        <v>63</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="27.6">
       <c r="A49" s="6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D49" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="E49" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5">
+        <v>68</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F49" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50" s="7"/>
       <c r="B50" s="7"/>
       <c r="C50" s="4"/>
       <c r="D50" s="7"/>
-      <c r="E50" s="10"/>
-    </row>
-    <row r="51" spans="1:5" ht="16" thickBot="1">
+      <c r="E50" s="7"/>
+      <c r="F50" s="7"/>
+    </row>
+    <row r="51" spans="1:6" ht="15" thickBot="1">
       <c r="A51" s="8"/>
       <c r="B51" s="8"/>
       <c r="C51" s="2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D51" s="8"/>
-      <c r="E51" s="11"/>
-    </row>
-    <row r="52" spans="1:5" ht="46" thickBot="1">
+      <c r="E51" s="8"/>
+      <c r="F51" s="8"/>
+    </row>
+    <row r="52" spans="1:6" ht="42" thickBot="1">
       <c r="A52" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E52" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5">
+        <v>72</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
       <c r="A53" s="5"/>
       <c r="B53" s="5"/>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="5"/>
-    </row>
-    <row r="54" spans="1:5" ht="16" thickBot="1">
+      <c r="F53" s="5"/>
+    </row>
+    <row r="54" spans="1:6" ht="15" thickBot="1">
       <c r="A54" s="5"/>
       <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
+      <c r="C54" s="5" t="s">
+        <v>146</v>
+      </c>
       <c r="D54" s="5"/>
       <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" ht="16" thickBot="1">
+      <c r="F54" s="5"/>
+    </row>
+    <row r="55" spans="1:6" ht="15" thickBot="1">
       <c r="A55" s="3" t="s">
         <v>0</v>
       </c>
@@ -1864,106 +1933,127 @@
       <c r="E55" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" ht="81.5" customHeight="1">
+      <c r="F55" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="81.599999999999994" customHeight="1">
       <c r="A56" s="6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="D56" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="E56" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
+        <v>137</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F56" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
       <c r="A57" s="7"/>
       <c r="B57" s="7"/>
       <c r="C57" s="4"/>
       <c r="D57" s="7"/>
-      <c r="E57" s="10"/>
-    </row>
-    <row r="58" spans="1:5" ht="31" thickBot="1">
+      <c r="E57" s="7"/>
+      <c r="F57" s="7"/>
+    </row>
+    <row r="58" spans="1:6" ht="28.2" thickBot="1">
       <c r="A58" s="8"/>
       <c r="B58" s="8"/>
       <c r="C58" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D58" s="8"/>
-      <c r="E58" s="11"/>
-    </row>
-    <row r="59" spans="1:5" ht="46" thickBot="1">
+      <c r="E58" s="8"/>
+      <c r="F58" s="8"/>
+    </row>
+    <row r="59" spans="1:6" ht="42" thickBot="1">
       <c r="A59" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="E59" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="46" thickBot="1">
+        <v>80</v>
+      </c>
+      <c r="E59" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F59" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="42" thickBot="1">
       <c r="A60" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E60" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="46" thickBot="1">
+        <v>138</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="42" thickBot="1">
       <c r="A61" s="3" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="E61" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5">
+        <v>87</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
       <c r="A62" s="5"/>
       <c r="B62" s="5"/>
       <c r="C62" s="5"/>
       <c r="D62" s="5"/>
       <c r="E62" s="5"/>
-    </row>
-    <row r="63" spans="1:5" ht="16" thickBot="1">
+      <c r="F62" s="5"/>
+    </row>
+    <row r="63" spans="1:6" ht="15" thickBot="1">
       <c r="A63" s="5"/>
       <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
+      <c r="C63" s="5" t="s">
+        <v>147</v>
+      </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5"/>
-    </row>
-    <row r="64" spans="1:5" ht="16" thickBot="1">
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" spans="1:6" ht="15" thickBot="1">
       <c r="A64" s="3" t="s">
         <v>0</v>
       </c>
@@ -1979,105 +2069,125 @@
       <c r="E64" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="65" spans="1:5">
+      <c r="F64" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6">
       <c r="A65" s="6" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D65" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="E65" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5">
+        <v>92</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F65" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6">
       <c r="A66" s="7"/>
       <c r="B66" s="7"/>
       <c r="C66" s="4"/>
       <c r="D66" s="7"/>
-      <c r="E66" s="10"/>
-    </row>
-    <row r="67" spans="1:5" ht="16" thickBot="1">
+      <c r="E66" s="7"/>
+      <c r="F66" s="7"/>
+    </row>
+    <row r="67" spans="1:6" ht="15" thickBot="1">
       <c r="A67" s="8"/>
       <c r="B67" s="8"/>
       <c r="C67" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D67" s="8"/>
-      <c r="E67" s="11"/>
-    </row>
-    <row r="68" spans="1:5" ht="30">
+      <c r="E67" s="8"/>
+      <c r="F67" s="8"/>
+    </row>
+    <row r="68" spans="1:6" ht="27.6">
       <c r="A68" s="6" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="D68" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="E68" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5">
+        <v>139</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F68" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6">
       <c r="A69" s="7"/>
       <c r="B69" s="7"/>
       <c r="C69" s="4"/>
       <c r="D69" s="7"/>
-      <c r="E69" s="10"/>
-    </row>
-    <row r="70" spans="1:5" ht="16" thickBot="1">
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+    </row>
+    <row r="70" spans="1:6" ht="15" thickBot="1">
       <c r="A70" s="8"/>
       <c r="B70" s="8"/>
       <c r="C70" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D70" s="8"/>
-      <c r="E70" s="11"/>
-    </row>
-    <row r="71" spans="1:5" ht="46" thickBot="1">
+      <c r="E70" s="8"/>
+      <c r="F70" s="8"/>
+    </row>
+    <row r="71" spans="1:6" ht="42" thickBot="1">
       <c r="A71" s="3" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E71" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5">
+        <v>140</v>
+      </c>
+      <c r="E71" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6">
       <c r="A72" s="5"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
       <c r="E72" s="5"/>
-    </row>
-    <row r="73" spans="1:5" ht="16" thickBot="1">
+      <c r="F72" s="5"/>
+    </row>
+    <row r="73" spans="1:6" ht="15" thickBot="1">
       <c r="A73" s="5"/>
       <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
+      <c r="C73" s="5" t="s">
+        <v>148</v>
+      </c>
       <c r="D73" s="5"/>
       <c r="E73" s="5"/>
-    </row>
-    <row r="74" spans="1:5" ht="16" thickBot="1">
+      <c r="F73" s="5"/>
+    </row>
+    <row r="74" spans="1:6" ht="15" thickBot="1">
       <c r="A74" s="3" t="s">
         <v>0</v>
       </c>
@@ -2093,105 +2203,125 @@
       <c r="E74" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:5">
+      <c r="F74" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6">
       <c r="A75" s="6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D75" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E75" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
+        <v>104</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F75" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6">
       <c r="A76" s="7"/>
       <c r="B76" s="7"/>
       <c r="C76" s="4"/>
       <c r="D76" s="7"/>
-      <c r="E76" s="10"/>
-    </row>
-    <row r="77" spans="1:5" ht="31" thickBot="1">
+      <c r="E76" s="7"/>
+      <c r="F76" s="7"/>
+    </row>
+    <row r="77" spans="1:6" ht="28.2" thickBot="1">
       <c r="A77" s="8"/>
       <c r="B77" s="8"/>
       <c r="C77" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="D77" s="8"/>
-      <c r="E77" s="11"/>
-    </row>
-    <row r="78" spans="1:5" ht="95.5" customHeight="1">
+      <c r="E77" s="8"/>
+      <c r="F77" s="8"/>
+    </row>
+    <row r="78" spans="1:6" ht="95.4" customHeight="1">
       <c r="A78" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D78" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="E78" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
+        <v>109</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6">
       <c r="A79" s="7"/>
       <c r="B79" s="7"/>
       <c r="C79" s="4"/>
       <c r="D79" s="7"/>
-      <c r="E79" s="10"/>
-    </row>
-    <row r="80" spans="1:5" ht="16" thickBot="1">
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+    </row>
+    <row r="80" spans="1:6" ht="15" thickBot="1">
       <c r="A80" s="8"/>
       <c r="B80" s="8"/>
       <c r="C80" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D80" s="8"/>
-      <c r="E80" s="11"/>
-    </row>
-    <row r="81" spans="1:5" ht="46" thickBot="1">
+      <c r="E80" s="8"/>
+      <c r="F80" s="8"/>
+    </row>
+    <row r="81" spans="1:6" ht="42" thickBot="1">
       <c r="A81" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="E81" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:5">
+        <v>112</v>
+      </c>
+      <c r="E81" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6">
       <c r="A82" s="5"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="5"/>
-    </row>
-    <row r="83" spans="1:5" ht="16" thickBot="1">
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" spans="1:6" ht="15" thickBot="1">
       <c r="A83" s="5"/>
       <c r="B83" s="5"/>
-      <c r="C83" s="5"/>
+      <c r="C83" s="5" t="s">
+        <v>149</v>
+      </c>
       <c r="D83" s="5"/>
       <c r="E83" s="5"/>
-    </row>
-    <row r="84" spans="1:5" ht="16" thickBot="1">
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" spans="1:6" ht="15" thickBot="1">
       <c r="A84" s="3" t="s">
         <v>0</v>
       </c>
@@ -2207,172 +2337,208 @@
       <c r="E84" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" ht="46" thickBot="1">
+      <c r="F84" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="42" thickBot="1">
       <c r="A85" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B85" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="E85" s="12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="54" customHeight="1">
+        <v>116</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="54" customHeight="1">
       <c r="A86" s="6" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E86" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5">
+        <v>121</v>
+      </c>
+      <c r="E86" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="F86" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6">
       <c r="A87" s="7"/>
       <c r="B87" s="7"/>
       <c r="C87" s="4"/>
       <c r="D87" s="7"/>
-      <c r="E87" s="10"/>
-    </row>
-    <row r="88" spans="1:5" ht="16" thickBot="1">
+      <c r="E87" s="7"/>
+      <c r="F87" s="7"/>
+    </row>
+    <row r="88" spans="1:6" ht="15" thickBot="1">
       <c r="A88" s="8"/>
       <c r="B88" s="8"/>
       <c r="C88" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D88" s="8"/>
-      <c r="E88" s="11"/>
-    </row>
-    <row r="89" spans="1:5" ht="30" customHeight="1">
+      <c r="E88" s="8"/>
+      <c r="F88" s="8"/>
+    </row>
+    <row r="89" spans="1:6" ht="27.6">
       <c r="A89" s="6" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="E89" s="9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5">
+        <v>125</v>
+      </c>
+      <c r="E89" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="F89" s="6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6">
       <c r="A90" s="7"/>
       <c r="B90" s="7"/>
       <c r="C90" s="4"/>
       <c r="D90" s="7"/>
-      <c r="E90" s="10"/>
-    </row>
-    <row r="91" spans="1:5" ht="16" thickBot="1">
+      <c r="E90" s="7"/>
+      <c r="F90" s="7"/>
+    </row>
+    <row r="91" spans="1:6" ht="15" thickBot="1">
       <c r="A91" s="8"/>
       <c r="B91" s="8"/>
       <c r="C91" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D91" s="8"/>
-      <c r="E91" s="11"/>
+      <c r="E91" s="8"/>
+      <c r="F91" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="80">
+  <mergeCells count="100">
+    <mergeCell ref="A86:A88"/>
+    <mergeCell ref="B86:B88"/>
+    <mergeCell ref="D86:D88"/>
+    <mergeCell ref="E86:E88"/>
+    <mergeCell ref="F86:F88"/>
+    <mergeCell ref="A89:A91"/>
+    <mergeCell ref="B89:B91"/>
+    <mergeCell ref="D89:D91"/>
+    <mergeCell ref="E89:E91"/>
+    <mergeCell ref="F89:F91"/>
+    <mergeCell ref="A75:A77"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="D75:D77"/>
+    <mergeCell ref="E75:E77"/>
+    <mergeCell ref="F75:F77"/>
+    <mergeCell ref="A78:A80"/>
+    <mergeCell ref="B78:B80"/>
+    <mergeCell ref="D78:D80"/>
+    <mergeCell ref="E78:E80"/>
+    <mergeCell ref="F78:F80"/>
+    <mergeCell ref="A65:A67"/>
+    <mergeCell ref="B65:B67"/>
+    <mergeCell ref="D65:D67"/>
+    <mergeCell ref="E65:E67"/>
+    <mergeCell ref="F65:F67"/>
+    <mergeCell ref="A68:A70"/>
+    <mergeCell ref="B68:B70"/>
+    <mergeCell ref="D68:D70"/>
+    <mergeCell ref="E68:E70"/>
+    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="D49:D51"/>
+    <mergeCell ref="E49:E51"/>
+    <mergeCell ref="F49:F51"/>
+    <mergeCell ref="A56:A58"/>
+    <mergeCell ref="B56:B58"/>
+    <mergeCell ref="D56:D58"/>
+    <mergeCell ref="E56:E58"/>
+    <mergeCell ref="F56:F58"/>
+    <mergeCell ref="A39:A41"/>
+    <mergeCell ref="B39:B41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="A45:A47"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="D45:D47"/>
+    <mergeCell ref="E45:E47"/>
+    <mergeCell ref="F45:F47"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="E33:E35"/>
+    <mergeCell ref="F33:F35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="E36:E38"/>
+    <mergeCell ref="F36:F38"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="E24:E26"/>
+    <mergeCell ref="F24:F26"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="D30:D32"/>
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="F30:F32"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="B21:B23"/>
+    <mergeCell ref="D21:D23"/>
+    <mergeCell ref="E21:E23"/>
+    <mergeCell ref="F21:F23"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="D8:D10"/>
+    <mergeCell ref="E8:E10"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="F15:F17"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="D2:D4"/>
+    <mergeCell ref="E2:E4"/>
+    <mergeCell ref="F2:F4"/>
     <mergeCell ref="A5:A7"/>
     <mergeCell ref="B5:B7"/>
     <mergeCell ref="D5:D7"/>
     <mergeCell ref="E5:E7"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="E2:E4"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="E15:E17"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="D8:D10"/>
-    <mergeCell ref="E8:E10"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="D21:D23"/>
-    <mergeCell ref="E21:E23"/>
-    <mergeCell ref="A18:A20"/>
-    <mergeCell ref="B18:B20"/>
-    <mergeCell ref="D18:D20"/>
-    <mergeCell ref="E18:E20"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="D30:D32"/>
-    <mergeCell ref="E30:E32"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="E24:E26"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="D36:D38"/>
-    <mergeCell ref="E36:E38"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="D33:D35"/>
-    <mergeCell ref="E33:E35"/>
-    <mergeCell ref="A45:A47"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="D45:D47"/>
-    <mergeCell ref="E45:E47"/>
-    <mergeCell ref="A39:A41"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="A56:A58"/>
-    <mergeCell ref="B56:B58"/>
-    <mergeCell ref="D56:D58"/>
-    <mergeCell ref="E56:E58"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="D49:D51"/>
-    <mergeCell ref="E49:E51"/>
-    <mergeCell ref="A68:A70"/>
-    <mergeCell ref="B68:B70"/>
-    <mergeCell ref="D68:D70"/>
-    <mergeCell ref="E68:E70"/>
-    <mergeCell ref="A65:A67"/>
-    <mergeCell ref="B65:B67"/>
-    <mergeCell ref="D65:D67"/>
-    <mergeCell ref="E65:E67"/>
-    <mergeCell ref="A78:A80"/>
-    <mergeCell ref="B78:B80"/>
-    <mergeCell ref="D78:D80"/>
-    <mergeCell ref="E78:E80"/>
-    <mergeCell ref="A75:A77"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="D75:D77"/>
-    <mergeCell ref="E75:E77"/>
-    <mergeCell ref="A89:A91"/>
-    <mergeCell ref="B89:B91"/>
-    <mergeCell ref="D89:D91"/>
-    <mergeCell ref="E89:E91"/>
-    <mergeCell ref="A86:A88"/>
-    <mergeCell ref="B86:B88"/>
-    <mergeCell ref="D86:D88"/>
-    <mergeCell ref="E86:E88"/>
+    <mergeCell ref="F5:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>